<commit_message>
Local Date with moment
</commit_message>
<xml_diff>
--- a/dailyreport.xlsx
+++ b/dailyreport.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="34">
   <si>
     <t>일자</t>
   </si>
   <si>
-    <t>2019-12-08</t>
+    <t>2019-12-09</t>
   </si>
   <si>
     <t>시간</t>
@@ -87,55 +87,37 @@
     <t>1-2</t>
   </si>
   <si>
-    <t>00:19:52</t>
-  </si>
-  <si>
-    <t>00:33:35</t>
-  </si>
-  <si>
     <t>2-3</t>
   </si>
   <si>
-    <t>00:31:47</t>
-  </si>
-  <si>
-    <t>01:00:00</t>
-  </si>
-  <si>
     <t>3-4</t>
   </si>
   <si>
-    <t>00:31:50</t>
-  </si>
-  <si>
     <t>4-5</t>
   </si>
   <si>
-    <t>00:30:53</t>
-  </si>
-  <si>
     <t>5-6</t>
   </si>
   <si>
-    <t>00:30:54</t>
-  </si>
-  <si>
     <t>6-7</t>
   </si>
   <si>
-    <t>00:30:55</t>
-  </si>
-  <si>
     <t>7-8</t>
   </si>
   <si>
-    <t>00:24:46</t>
-  </si>
-  <si>
-    <t>00:53:32</t>
+    <t>00:14:13</t>
+  </si>
+  <si>
+    <t>00:31:38</t>
   </si>
   <si>
     <t>8-9</t>
+  </si>
+  <si>
+    <t>00:22:53</t>
+  </si>
+  <si>
+    <t>00:46:59</t>
   </si>
   <si>
     <t>9-10</t>
@@ -936,716 +918,716 @@
         <v>21</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="12">
-        <v>29.32</v>
+        <v>19</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="12">
-        <v>21.17</v>
-      </c>
-      <c r="F5" s="12">
-        <v>126</v>
-      </c>
-      <c r="G5" s="12">
-        <v>10.89</v>
-      </c>
-      <c r="H5" s="12">
-        <v>13.89</v>
-      </c>
-      <c r="I5" s="12">
-        <v>90.28</v>
-      </c>
-      <c r="J5" s="12">
-        <v>5.78</v>
-      </c>
-      <c r="K5" s="12">
-        <v>11.6</v>
-      </c>
-      <c r="L5" s="12">
-        <v>107.67</v>
-      </c>
-      <c r="M5" s="12">
-        <v>10.28</v>
-      </c>
-      <c r="N5" s="12">
-        <v>17.86</v>
-      </c>
-      <c r="O5" s="12">
-        <v>232.4</v>
-      </c>
-      <c r="P5" s="12">
-        <v>13.61</v>
-      </c>
-      <c r="Q5" s="12">
-        <v>17.88</v>
-      </c>
-      <c r="R5" s="12">
-        <v>105.62</v>
-      </c>
-      <c r="S5" s="12">
-        <v>10.69</v>
-      </c>
-      <c r="T5" s="12">
-        <v>12.61</v>
-      </c>
-      <c r="U5" s="12">
-        <v>131.41</v>
-      </c>
-      <c r="V5" s="12">
-        <v>14.24</v>
-      </c>
-      <c r="W5" s="12">
-        <v>14.87</v>
-      </c>
-      <c r="X5" s="12">
-        <v>227.2</v>
-      </c>
-      <c r="Y5" s="12">
-        <v>12.84</v>
-      </c>
-      <c r="Z5" s="12">
-        <v>15.74</v>
-      </c>
-      <c r="AA5" s="12">
-        <v>147.77</v>
-      </c>
-      <c r="AB5" s="12">
-        <v>7.76</v>
-      </c>
-      <c r="AC5" s="13">
-        <v>10.72</v>
+        <v>19</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="U5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="V5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="W5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="X5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC5" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="12">
-        <v>31.49</v>
+        <v>19</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="12">
-        <v>21.83</v>
-      </c>
-      <c r="F6" s="12">
-        <v>115.27</v>
-      </c>
-      <c r="G6" s="12">
-        <v>6</v>
-      </c>
-      <c r="H6" s="12">
-        <v>12.64</v>
-      </c>
-      <c r="I6" s="12">
-        <v>12.64</v>
-      </c>
-      <c r="J6" s="12">
-        <v>7.58</v>
-      </c>
-      <c r="K6" s="12">
-        <v>10.36</v>
-      </c>
-      <c r="L6" s="12">
-        <v>109.58</v>
-      </c>
-      <c r="M6" s="12">
-        <v>9.04</v>
-      </c>
-      <c r="N6" s="12">
-        <v>14.28</v>
-      </c>
-      <c r="O6" s="12">
-        <v>24.29</v>
-      </c>
-      <c r="P6" s="12">
-        <v>13.51</v>
-      </c>
-      <c r="Q6" s="12">
-        <v>17.95</v>
-      </c>
-      <c r="R6" s="12">
-        <v>14.32</v>
-      </c>
-      <c r="S6" s="12">
-        <v>10.79</v>
-      </c>
-      <c r="T6" s="12">
-        <v>12.29</v>
-      </c>
-      <c r="U6" s="12">
-        <v>15.39</v>
-      </c>
-      <c r="V6" s="12">
-        <v>14.09</v>
-      </c>
-      <c r="W6" s="12">
-        <v>14.73</v>
-      </c>
-      <c r="X6" s="12">
-        <v>16.73</v>
-      </c>
-      <c r="Y6" s="12">
-        <v>15.31</v>
-      </c>
-      <c r="Z6" s="12">
-        <v>16.01</v>
-      </c>
-      <c r="AA6" s="12">
-        <v>11.53</v>
-      </c>
-      <c r="AB6" s="12">
-        <v>10.55</v>
-      </c>
-      <c r="AC6" s="13">
-        <v>11.04</v>
+        <v>19</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="V6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="W6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="X6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC6" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="12">
-        <v>31.43</v>
+        <v>19</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="12">
-        <v>21.82</v>
-      </c>
-      <c r="F7" s="12">
-        <v>119.14</v>
-      </c>
-      <c r="G7" s="12">
-        <v>10.1</v>
-      </c>
-      <c r="H7" s="12">
-        <v>12.86</v>
-      </c>
-      <c r="I7" s="12">
-        <v>12.43</v>
-      </c>
-      <c r="J7" s="12">
-        <v>7.32</v>
-      </c>
-      <c r="K7" s="12">
-        <v>10.05</v>
-      </c>
-      <c r="L7" s="12">
-        <v>108.4</v>
-      </c>
-      <c r="M7" s="12">
-        <v>9.91</v>
-      </c>
-      <c r="N7" s="12">
-        <v>13.28</v>
-      </c>
-      <c r="O7" s="12">
-        <v>23.81</v>
-      </c>
-      <c r="P7" s="12">
-        <v>13.38</v>
-      </c>
-      <c r="Q7" s="12">
-        <v>17.92</v>
-      </c>
-      <c r="R7" s="12">
-        <v>13.77</v>
-      </c>
-      <c r="S7" s="12">
-        <v>10.29</v>
-      </c>
-      <c r="T7" s="12">
-        <v>12.09</v>
-      </c>
-      <c r="U7" s="12">
-        <v>15.33</v>
-      </c>
-      <c r="V7" s="12">
-        <v>13.78</v>
-      </c>
-      <c r="W7" s="12">
-        <v>14.75</v>
-      </c>
-      <c r="X7" s="12">
-        <v>16.58</v>
-      </c>
-      <c r="Y7" s="12">
-        <v>15.35</v>
-      </c>
-      <c r="Z7" s="12">
-        <v>16.06</v>
-      </c>
-      <c r="AA7" s="12">
-        <v>11.77</v>
-      </c>
-      <c r="AB7" s="12">
-        <v>10.7</v>
-      </c>
-      <c r="AC7" s="13">
-        <v>11.21</v>
+        <v>19</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC7" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="12">
-        <v>31.53</v>
+        <v>19</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="12">
-        <v>21.82</v>
-      </c>
-      <c r="F8" s="12">
-        <v>110.76</v>
-      </c>
-      <c r="G8" s="12">
-        <v>0.61</v>
-      </c>
-      <c r="H8" s="12">
-        <v>12.57</v>
-      </c>
-      <c r="I8" s="12">
-        <v>12.31</v>
-      </c>
-      <c r="J8" s="12">
-        <v>7.14</v>
-      </c>
-      <c r="K8" s="12">
-        <v>9.8</v>
-      </c>
-      <c r="L8" s="12">
-        <v>110.94</v>
-      </c>
-      <c r="M8" s="12">
-        <v>8.14</v>
-      </c>
-      <c r="N8" s="12">
-        <v>12.22</v>
-      </c>
-      <c r="O8" s="12">
-        <v>26.27</v>
-      </c>
-      <c r="P8" s="12">
-        <v>13.4</v>
-      </c>
-      <c r="Q8" s="12">
-        <v>17.88</v>
-      </c>
-      <c r="R8" s="12">
-        <v>13.65</v>
-      </c>
-      <c r="S8" s="12">
-        <v>10.47</v>
-      </c>
-      <c r="T8" s="12">
-        <v>11.81</v>
-      </c>
-      <c r="U8" s="12">
-        <v>15.27</v>
-      </c>
-      <c r="V8" s="12">
-        <v>13.86</v>
-      </c>
-      <c r="W8" s="12">
-        <v>14.75</v>
-      </c>
-      <c r="X8" s="12">
-        <v>16.97</v>
-      </c>
-      <c r="Y8" s="12">
-        <v>15.6</v>
-      </c>
-      <c r="Z8" s="12">
-        <v>16.23</v>
-      </c>
-      <c r="AA8" s="12">
-        <v>11.97</v>
-      </c>
-      <c r="AB8" s="12">
-        <v>10.62</v>
-      </c>
-      <c r="AC8" s="13">
-        <v>11.29</v>
+        <v>19</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="U8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="V8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="W8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="X8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC8" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="12">
-        <v>31.48</v>
+        <v>19</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="12">
-        <v>21.82</v>
-      </c>
-      <c r="F9" s="12">
-        <v>116.55</v>
-      </c>
-      <c r="G9" s="12">
-        <v>9.78</v>
-      </c>
-      <c r="H9" s="12">
-        <v>12.67</v>
-      </c>
-      <c r="I9" s="12">
-        <v>12.2</v>
-      </c>
-      <c r="J9" s="12">
-        <v>7.32</v>
-      </c>
-      <c r="K9" s="12">
-        <v>9.72</v>
-      </c>
-      <c r="L9" s="12">
-        <v>103.25</v>
-      </c>
-      <c r="M9" s="12">
-        <v>8.43</v>
-      </c>
-      <c r="N9" s="12">
-        <v>12.13</v>
-      </c>
-      <c r="O9" s="12">
-        <v>26.32</v>
-      </c>
-      <c r="P9" s="12">
-        <v>13.19</v>
-      </c>
-      <c r="Q9" s="12">
-        <v>17.76</v>
-      </c>
-      <c r="R9" s="12">
-        <v>13.94</v>
-      </c>
-      <c r="S9" s="12">
-        <v>10.42</v>
-      </c>
-      <c r="T9" s="12">
-        <v>11.75</v>
-      </c>
-      <c r="U9" s="12">
-        <v>15.59</v>
-      </c>
-      <c r="V9" s="12">
-        <v>14.13</v>
-      </c>
-      <c r="W9" s="12">
-        <v>14.8</v>
-      </c>
-      <c r="X9" s="12">
-        <v>16.73</v>
-      </c>
-      <c r="Y9" s="12">
-        <v>15.2</v>
-      </c>
-      <c r="Z9" s="12">
-        <v>15.97</v>
-      </c>
-      <c r="AA9" s="12">
-        <v>11.75</v>
-      </c>
-      <c r="AB9" s="12">
-        <v>10.59</v>
-      </c>
-      <c r="AC9" s="13">
-        <v>11.18</v>
+        <v>19</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="U9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="V9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="W9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="X9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC9" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="12">
-        <v>31.5</v>
+        <v>19</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="12">
-        <v>21.82</v>
-      </c>
-      <c r="F10" s="12">
-        <v>117.31</v>
-      </c>
-      <c r="G10" s="12">
-        <v>10.02</v>
-      </c>
-      <c r="H10" s="12">
-        <v>12.92</v>
-      </c>
-      <c r="I10" s="12">
-        <v>12.02</v>
-      </c>
-      <c r="J10" s="12">
-        <v>7.16</v>
-      </c>
-      <c r="K10" s="12">
-        <v>9.57</v>
-      </c>
-      <c r="L10" s="12">
-        <v>106.11</v>
-      </c>
-      <c r="M10" s="12">
-        <v>8.41</v>
-      </c>
-      <c r="N10" s="12">
-        <v>12.16</v>
-      </c>
-      <c r="O10" s="12">
-        <v>25.86</v>
-      </c>
-      <c r="P10" s="12">
-        <v>13.21</v>
-      </c>
-      <c r="Q10" s="12">
-        <v>17.63</v>
-      </c>
-      <c r="R10" s="12">
-        <v>13.66</v>
-      </c>
-      <c r="S10" s="12">
-        <v>10.45</v>
-      </c>
-      <c r="T10" s="12">
-        <v>11.75</v>
-      </c>
-      <c r="U10" s="12">
-        <v>15.86</v>
-      </c>
-      <c r="V10" s="12">
-        <v>14.08</v>
-      </c>
-      <c r="W10" s="12">
-        <v>14.74</v>
-      </c>
-      <c r="X10" s="12">
-        <v>16.68</v>
-      </c>
-      <c r="Y10" s="12">
-        <v>15</v>
-      </c>
-      <c r="Z10" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="AA10" s="12">
-        <v>11.65</v>
-      </c>
-      <c r="AB10" s="12">
-        <v>10.55</v>
-      </c>
-      <c r="AC10" s="13">
-        <v>11.17</v>
+        <v>19</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="R10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="T10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="U10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="V10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="W10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="X10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC10" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C11" s="12">
-        <v>31.46</v>
+        <v>30.44</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E11" s="12">
-        <v>21.78</v>
+        <v>16.57</v>
       </c>
       <c r="F11" s="12">
-        <v>109.56</v>
+        <v>131.99</v>
       </c>
       <c r="G11" s="12">
-        <v>8.8</v>
+        <v>8.86</v>
       </c>
       <c r="H11" s="12">
-        <v>12.96</v>
+        <v>13.87</v>
       </c>
       <c r="I11" s="12">
-        <v>77.55</v>
+        <v>89.48</v>
       </c>
       <c r="J11" s="12">
-        <v>6.73</v>
+        <v>5.77</v>
       </c>
       <c r="K11" s="12">
-        <v>9.5</v>
+        <v>11.67</v>
       </c>
       <c r="L11" s="12">
-        <v>108.57</v>
+        <v>110.25</v>
       </c>
       <c r="M11" s="12">
-        <v>4.28</v>
+        <v>6.17</v>
       </c>
       <c r="N11" s="12">
-        <v>12.23</v>
+        <v>13.51</v>
       </c>
       <c r="O11" s="12">
-        <v>25.71</v>
+        <v>219.09</v>
       </c>
       <c r="P11" s="12">
-        <v>13.34</v>
+        <v>13.23</v>
       </c>
       <c r="Q11" s="12">
-        <v>17.62</v>
+        <v>17.96</v>
       </c>
       <c r="R11" s="12">
-        <v>13.65</v>
+        <v>106.73</v>
       </c>
       <c r="S11" s="12">
-        <v>10.21</v>
+        <v>10.45</v>
       </c>
       <c r="T11" s="12">
-        <v>11.68</v>
+        <v>12.29</v>
       </c>
       <c r="U11" s="12">
-        <v>15.47</v>
+        <v>128.63</v>
       </c>
       <c r="V11" s="12">
-        <v>13.78</v>
+        <v>14.53</v>
       </c>
       <c r="W11" s="12">
-        <v>14.72</v>
+        <v>15.03</v>
       </c>
       <c r="X11" s="12">
-        <v>16.4</v>
+        <v>236.79</v>
       </c>
       <c r="Y11" s="12">
-        <v>14.22</v>
+        <v>13.2</v>
       </c>
       <c r="Z11" s="12">
-        <v>15.7</v>
+        <v>14.53</v>
       </c>
       <c r="AA11" s="12">
-        <v>11.76</v>
+        <v>147.12</v>
       </c>
       <c r="AB11" s="12">
-        <v>9.11</v>
+        <v>8.08</v>
       </c>
       <c r="AC11" s="13">
-        <v>11.04</v>
+        <v>9.66</v>
       </c>
     </row>
     <row r="12" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>20</v>
+        <v>31</v>
+      </c>
+      <c r="C12" s="12">
+        <v>32.01</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="P12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>20</v>
+        <v>32</v>
+      </c>
+      <c r="E12" s="12">
+        <v>18.88</v>
+      </c>
+      <c r="F12" s="12">
+        <v>117.95</v>
+      </c>
+      <c r="G12" s="12">
+        <v>7.54</v>
+      </c>
+      <c r="H12" s="12">
+        <v>11.33</v>
+      </c>
+      <c r="I12" s="12">
+        <v>79.65</v>
+      </c>
+      <c r="J12" s="12">
+        <v>7.47</v>
+      </c>
+      <c r="K12" s="12">
+        <v>10.69</v>
+      </c>
+      <c r="L12" s="12">
+        <v>101.91</v>
+      </c>
+      <c r="M12" s="12">
+        <v>9.02</v>
+      </c>
+      <c r="N12" s="12">
+        <v>12.98</v>
+      </c>
+      <c r="O12" s="12">
+        <v>27.84</v>
+      </c>
+      <c r="P12" s="12">
+        <v>12.86</v>
+      </c>
+      <c r="Q12" s="12">
+        <v>16.86</v>
       </c>
       <c r="R12" s="12">
-        <v>13.38</v>
+        <v>14.05</v>
       </c>
       <c r="S12" s="12">
-        <v>10.88</v>
+        <v>10.01</v>
       </c>
       <c r="T12" s="12">
-        <v>11.98</v>
+        <v>12.07</v>
       </c>
       <c r="U12" s="12">
-        <v>15.09</v>
+        <v>15.47</v>
       </c>
       <c r="V12" s="12">
-        <v>14.24</v>
+        <v>13.93</v>
       </c>
       <c r="W12" s="12">
-        <v>14.55</v>
+        <v>14.83</v>
       </c>
       <c r="X12" s="12">
-        <v>14.72</v>
+        <v>15.68</v>
       </c>
       <c r="Y12" s="12">
-        <v>13.93</v>
+        <v>13.07</v>
       </c>
       <c r="Z12" s="12">
-        <v>14.34</v>
+        <v>14.81</v>
       </c>
       <c r="AA12" s="12">
-        <v>10.38</v>
+        <v>11.46</v>
       </c>
       <c r="AB12" s="12">
-        <v>8.08</v>
+        <v>8.5</v>
       </c>
       <c r="AC12" s="13">
-        <v>8.98</v>
+        <v>10.58</v>
       </c>
     </row>
     <row r="13" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>19</v>
@@ -1659,77 +1641,77 @@
       <c r="E13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="P13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="R13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="S13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="T13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="U13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="V13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="W13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="X13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC13" s="13" t="s">
-        <v>20</v>
+      <c r="F13" s="12">
+        <v>7.79</v>
+      </c>
+      <c r="G13" s="12">
+        <v>7.79</v>
+      </c>
+      <c r="H13" s="12">
+        <v>7.79</v>
+      </c>
+      <c r="I13" s="12">
+        <v>11.03</v>
+      </c>
+      <c r="J13" s="12">
+        <v>11.03</v>
+      </c>
+      <c r="K13" s="12">
+        <v>11.03</v>
+      </c>
+      <c r="L13" s="12">
+        <v>10.95</v>
+      </c>
+      <c r="M13" s="12">
+        <v>10.95</v>
+      </c>
+      <c r="N13" s="12">
+        <v>10.95</v>
+      </c>
+      <c r="O13" s="12">
+        <v>13.64</v>
+      </c>
+      <c r="P13" s="12">
+        <v>13.64</v>
+      </c>
+      <c r="Q13" s="12">
+        <v>13.64</v>
+      </c>
+      <c r="R13" s="12">
+        <v>11.48</v>
+      </c>
+      <c r="S13" s="12">
+        <v>11.48</v>
+      </c>
+      <c r="T13" s="12">
+        <v>11.48</v>
+      </c>
+      <c r="U13" s="12">
+        <v>14.49</v>
+      </c>
+      <c r="V13" s="12">
+        <v>14.49</v>
+      </c>
+      <c r="W13" s="12">
+        <v>14.49</v>
+      </c>
+      <c r="X13" s="12">
+        <v>13.2</v>
+      </c>
+      <c r="Y13" s="12">
+        <v>13.2</v>
+      </c>
+      <c r="Z13" s="12">
+        <v>13.2</v>
+      </c>
+      <c r="AA13" s="12">
+        <v>8.64</v>
+      </c>
+      <c r="AB13" s="12">
+        <v>8.64</v>
+      </c>
+      <c r="AC13" s="13">
+        <v>8.64</v>
       </c>
     </row>
     <row r="14" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>